<commit_message>
New documents and updates
</commit_message>
<xml_diff>
--- a/Documents/0 Project Managment/Project Plan - 2012.xlsx
+++ b/Documents/0 Project Managment/Project Plan - 2012.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="-15" yWindow="60" windowWidth="15120" windowHeight="1665"/>
+    <workbookView xWindow="-15" yWindow="120" windowWidth="15120" windowHeight="1605"/>
   </bookViews>
   <sheets>
     <sheet name="Detail plan Reduced Scope" sheetId="6" r:id="rId1"/>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="79">
   <si>
     <t>Who</t>
   </si>
@@ -170,9 +170,6 @@
     <t>Test</t>
   </si>
   <si>
-    <t>3/7</t>
-  </si>
-  <si>
     <t>Go Live</t>
   </si>
   <si>
@@ -207,6 +204,57 @@
   </si>
   <si>
     <t>Report bugs in Cloud AppStudio360</t>
+  </si>
+  <si>
+    <t>US5: Create Android template.</t>
+  </si>
+  <si>
+    <t>US6: Break down requirments</t>
+  </si>
+  <si>
+    <t>Scrum poker for estimate tasks</t>
+  </si>
+  <si>
+    <t>US7: Mitt Nya Hem - Bostadsformulär</t>
+  </si>
+  <si>
+    <t>US9: Ta fram team i mittNyaHem</t>
+  </si>
+  <si>
+    <t>US10: Utveckla en native Androidapp som konsumerar och visar information från Mitt Nya Hem.</t>
+  </si>
+  <si>
+    <t>US11: Open Id inloggning via Android</t>
+  </si>
+  <si>
+    <t>US12:  Använd OAUTH för att använda Google Docs som den påloggade användaren</t>
+  </si>
+  <si>
+    <t>US13: Skapa en Cloud App Studio app anpassad för Apple Retina skärmar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloud App </t>
+  </si>
+  <si>
+    <t>Android</t>
+  </si>
+  <si>
+    <t>Planning</t>
+  </si>
+  <si>
+    <t>Stablization</t>
+  </si>
+  <si>
+    <t>TEST Cloud App</t>
+  </si>
+  <si>
+    <t>US4: Documentation</t>
+  </si>
+  <si>
+    <t>TEST Android and Cloud app</t>
+  </si>
+  <si>
+    <t>5/27</t>
   </si>
 </sst>
 </file>
@@ -250,7 +298,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -287,8 +335,62 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor theme="0" tint="-0.14996795556505021"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39994506668294322"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor theme="0" tint="-0.14993743705557422"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -552,11 +654,52 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -617,7 +760,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -658,6 +800,15 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -666,13 +817,46 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -982,110 +1166,114 @@
   <dimension ref="A1:BN16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="AB3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Q5" sqref="Q5"/>
+      <selection pane="bottomRight" activeCell="AN12" sqref="AN12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="66" width="9.140625" style="3"/>
+    <col min="7" max="32" width="9.140625" style="3"/>
+    <col min="33" max="36" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="37" max="44" width="9.140625" style="3"/>
+    <col min="45" max="45" width="9.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="46" max="66" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:66" x14ac:dyDescent="0.25">
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="64"/>
-      <c r="G1" s="59" t="s">
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="E1" s="65"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="58" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="60"/>
-      <c r="I1" s="60"/>
-      <c r="J1" s="60"/>
-      <c r="K1" s="61"/>
-      <c r="L1" s="59" t="s">
+      <c r="H1" s="59"/>
+      <c r="I1" s="59"/>
+      <c r="J1" s="59"/>
+      <c r="K1" s="60"/>
+      <c r="L1" s="58" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="60"/>
-      <c r="N1" s="60"/>
-      <c r="O1" s="60"/>
-      <c r="P1" s="61"/>
-      <c r="Q1" s="59" t="s">
+      <c r="M1" s="59"/>
+      <c r="N1" s="59"/>
+      <c r="O1" s="59"/>
+      <c r="P1" s="60"/>
+      <c r="Q1" s="58" t="s">
         <v>5</v>
       </c>
-      <c r="R1" s="60"/>
-      <c r="S1" s="60"/>
-      <c r="T1" s="60"/>
-      <c r="U1" s="61"/>
-      <c r="V1" s="65" t="s">
+      <c r="R1" s="59"/>
+      <c r="S1" s="59"/>
+      <c r="T1" s="59"/>
+      <c r="U1" s="60"/>
+      <c r="V1" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="W1" s="66"/>
-      <c r="X1" s="66"/>
-      <c r="Y1" s="66"/>
-      <c r="Z1" s="67"/>
-      <c r="AA1" s="59" t="s">
+      <c r="W1" s="62"/>
+      <c r="X1" s="62"/>
+      <c r="Y1" s="62"/>
+      <c r="Z1" s="63"/>
+      <c r="AA1" s="58" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" s="60"/>
-      <c r="AC1" s="60"/>
-      <c r="AD1" s="60"/>
-      <c r="AE1" s="61"/>
-      <c r="AF1" s="59" t="s">
+      <c r="AB1" s="59"/>
+      <c r="AC1" s="59"/>
+      <c r="AD1" s="59"/>
+      <c r="AE1" s="60"/>
+      <c r="AF1" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="AG1" s="60"/>
-      <c r="AH1" s="60"/>
-      <c r="AI1" s="60"/>
-      <c r="AJ1" s="61"/>
-      <c r="AK1" s="59" t="s">
+      <c r="AG1" s="59"/>
+      <c r="AH1" s="59"/>
+      <c r="AI1" s="59"/>
+      <c r="AJ1" s="60"/>
+      <c r="AK1" s="58" t="s">
         <v>9</v>
       </c>
-      <c r="AL1" s="60"/>
-      <c r="AM1" s="60"/>
-      <c r="AN1" s="60"/>
-      <c r="AO1" s="61"/>
-      <c r="AP1" s="65" t="s">
+      <c r="AL1" s="59"/>
+      <c r="AM1" s="59"/>
+      <c r="AN1" s="59"/>
+      <c r="AO1" s="60"/>
+      <c r="AP1" s="61" t="s">
         <v>10</v>
       </c>
-      <c r="AQ1" s="66"/>
-      <c r="AR1" s="66"/>
-      <c r="AS1" s="66"/>
-      <c r="AT1" s="67"/>
-      <c r="AU1" s="59" t="s">
+      <c r="AQ1" s="62"/>
+      <c r="AR1" s="62"/>
+      <c r="AS1" s="62"/>
+      <c r="AT1" s="63"/>
+      <c r="AU1" s="58" t="s">
         <v>11</v>
       </c>
-      <c r="AV1" s="60"/>
-      <c r="AW1" s="60"/>
-      <c r="AX1" s="60"/>
-      <c r="AY1" s="61"/>
-      <c r="AZ1" s="59" t="s">
+      <c r="AV1" s="59"/>
+      <c r="AW1" s="59"/>
+      <c r="AX1" s="59"/>
+      <c r="AY1" s="60"/>
+      <c r="AZ1" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="BA1" s="60"/>
-      <c r="BB1" s="60"/>
-      <c r="BC1" s="60"/>
-      <c r="BD1" s="61"/>
-      <c r="BE1" s="59" t="s">
+      <c r="BA1" s="59"/>
+      <c r="BB1" s="59"/>
+      <c r="BC1" s="59"/>
+      <c r="BD1" s="60"/>
+      <c r="BE1" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="BF1" s="60"/>
-      <c r="BG1" s="60"/>
-      <c r="BH1" s="60"/>
-      <c r="BI1" s="61"/>
-      <c r="BJ1" s="59" t="s">
+      <c r="BF1" s="59"/>
+      <c r="BG1" s="59"/>
+      <c r="BH1" s="59"/>
+      <c r="BI1" s="60"/>
+      <c r="BJ1" s="58" t="s">
         <v>14</v>
       </c>
-      <c r="BK1" s="60"/>
-      <c r="BL1" s="60"/>
-      <c r="BM1" s="60"/>
-      <c r="BN1" s="61"/>
+      <c r="BK1" s="59"/>
+      <c r="BL1" s="59"/>
+      <c r="BM1" s="59"/>
+      <c r="BN1" s="60"/>
     </row>
     <row r="2" spans="1:66" s="1" customFormat="1" ht="12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -1359,16 +1547,16 @@
       <c r="BM3" s="2"/>
       <c r="BN3" s="2"/>
     </row>
-    <row r="4" spans="1:66" s="33" customFormat="1" ht="84" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:66" s="33" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>42</v>
       </c>
-      <c r="B4" s="53"/>
-      <c r="C4" s="53"/>
-      <c r="D4" s="54"/>
+      <c r="B4" s="52"/>
+      <c r="C4" s="52"/>
+      <c r="D4" s="53"/>
       <c r="E4" s="25"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="55"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="54"/>
       <c r="H4" s="7" t="s">
         <v>48</v>
       </c>
@@ -1378,54 +1566,114 @@
       <c r="J4" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="K4" s="48" t="s">
+      <c r="K4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="L4" s="48" t="s">
+      <c r="L4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="M4" s="48" t="s">
+      <c r="M4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="N4" s="48" t="s">
+      <c r="N4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="O4" s="48" t="s">
+      <c r="O4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="P4" s="48" t="s">
+      <c r="P4" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="Q4" s="39"/>
-      <c r="R4" s="39"/>
-      <c r="S4" s="39"/>
-      <c r="T4" s="39"/>
-      <c r="U4" s="39"/>
-      <c r="V4" s="39"/>
-      <c r="W4" s="25"/>
-      <c r="X4" s="39"/>
-      <c r="Y4" s="39"/>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="39"/>
-      <c r="AB4" s="39"/>
-      <c r="AC4" s="39"/>
-      <c r="AD4" s="39"/>
-      <c r="AE4" s="25"/>
-      <c r="AF4" s="39"/>
-      <c r="AG4" s="39"/>
-      <c r="AH4" s="39"/>
-      <c r="AI4" s="39"/>
-      <c r="AJ4" s="39"/>
-      <c r="AK4" s="39"/>
-      <c r="AL4" s="39"/>
-      <c r="AM4" s="25"/>
-      <c r="AN4" s="39"/>
-      <c r="AO4" s="39"/>
-      <c r="AP4" s="39"/>
-      <c r="AQ4" s="39"/>
-      <c r="AR4" s="39"/>
-      <c r="AS4" s="39"/>
-      <c r="AT4" s="39"/>
+      <c r="Q4" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="R4" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="S4" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="T4" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="U4" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="V4" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="W4" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="X4" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="Y4" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z4" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA4" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB4" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC4" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD4" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE4" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF4" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG4" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH4" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI4" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ4" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK4" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL4" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM4" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="AN4" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="AO4" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP4" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ4" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR4" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS4" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT4" s="80" t="s">
+        <v>50</v>
+      </c>
       <c r="AU4" s="25"/>
       <c r="AV4" s="39"/>
       <c r="AW4" s="39"/>
@@ -1453,10 +1701,10 @@
       </c>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
-      <c r="F5" s="52"/>
-      <c r="G5" s="52"/>
+      <c r="D5" s="51"/>
+      <c r="E5" s="51"/>
+      <c r="F5" s="51"/>
+      <c r="G5" s="51"/>
       <c r="H5" s="4" t="s">
         <v>45</v>
       </c>
@@ -1484,36 +1732,96 @@
       <c r="P5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="Q5" s="39"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="39"/>
-      <c r="U5" s="39"/>
-      <c r="V5" s="39"/>
-      <c r="W5" s="39"/>
-      <c r="X5" s="39"/>
-      <c r="Y5" s="39"/>
-      <c r="Z5" s="39"/>
-      <c r="AA5" s="39"/>
-      <c r="AB5" s="39"/>
-      <c r="AC5" s="39"/>
-      <c r="AD5" s="39"/>
-      <c r="AE5" s="39"/>
-      <c r="AF5" s="39"/>
-      <c r="AG5" s="39"/>
-      <c r="AH5" s="39"/>
-      <c r="AI5" s="39"/>
-      <c r="AJ5" s="39"/>
-      <c r="AK5" s="39"/>
-      <c r="AL5" s="39"/>
-      <c r="AM5" s="39"/>
-      <c r="AN5" s="39"/>
-      <c r="AO5" s="39"/>
-      <c r="AP5" s="39"/>
-      <c r="AQ5" s="39"/>
-      <c r="AR5" s="39"/>
-      <c r="AS5" s="39"/>
-      <c r="AT5" s="39"/>
+      <c r="Q5" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="R5" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="S5" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="T5" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="U5" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="V5" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="W5" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="X5" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="Y5" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="Z5" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="AA5" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB5" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="AC5" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="AD5" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="AE5" s="73" t="s">
+        <v>67</v>
+      </c>
+      <c r="AF5" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG5" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH5" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI5" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ5" s="78" t="s">
+        <v>74</v>
+      </c>
+      <c r="AK5" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL5" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="AM5" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN5" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="AO5" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="AP5" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ5" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR5" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS5" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT5" s="80" t="s">
+        <v>50</v>
+      </c>
       <c r="AU5" s="39"/>
       <c r="AV5" s="39"/>
       <c r="AW5" s="39"/>
@@ -1535,7 +1843,7 @@
       <c r="BM5" s="25"/>
       <c r="BN5" s="25"/>
     </row>
-    <row r="6" spans="1:66" s="33" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:66" s="33" customFormat="1" ht="144" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>44</v>
       </c>
@@ -1572,36 +1880,96 @@
       <c r="P6" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Q6" s="39"/>
-      <c r="R6" s="39"/>
-      <c r="S6" s="39"/>
-      <c r="T6" s="39"/>
-      <c r="U6" s="39"/>
-      <c r="V6" s="39"/>
-      <c r="W6" s="39"/>
-      <c r="X6" s="39"/>
-      <c r="Y6" s="39"/>
-      <c r="Z6" s="39"/>
-      <c r="AA6" s="39"/>
-      <c r="AB6" s="39"/>
-      <c r="AC6" s="39"/>
-      <c r="AD6" s="39"/>
-      <c r="AE6" s="39"/>
-      <c r="AF6" s="39"/>
-      <c r="AG6" s="39"/>
-      <c r="AH6" s="39"/>
-      <c r="AI6" s="39"/>
-      <c r="AJ6" s="39"/>
-      <c r="AK6" s="39"/>
-      <c r="AL6" s="39"/>
-      <c r="AM6" s="39"/>
-      <c r="AN6" s="39"/>
-      <c r="AO6" s="39"/>
-      <c r="AP6" s="39"/>
-      <c r="AQ6" s="39"/>
-      <c r="AR6" s="39"/>
-      <c r="AS6" s="39"/>
-      <c r="AT6" s="39"/>
+      <c r="Q6" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="R6" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="S6" s="47" t="s">
+        <v>47</v>
+      </c>
+      <c r="T6" s="68" t="s">
+        <v>64</v>
+      </c>
+      <c r="U6" s="68" t="s">
+        <v>63</v>
+      </c>
+      <c r="V6" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="W6" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="X6" s="5" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y6" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z6" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA6" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="AB6" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC6" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="AD6" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="AE6" s="74" t="s">
+        <v>68</v>
+      </c>
+      <c r="AF6" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG6" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="AH6" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI6" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="AJ6" s="77" t="s">
+        <v>75</v>
+      </c>
+      <c r="AK6" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="AL6" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="AM6" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN6" s="47" t="s">
+        <v>76</v>
+      </c>
+      <c r="AO6" s="79" t="s">
+        <v>70</v>
+      </c>
+      <c r="AP6" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="AQ6" s="73" t="s">
+        <v>69</v>
+      </c>
+      <c r="AR6" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="AS6" s="76" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT6" s="80" t="s">
+        <v>50</v>
+      </c>
       <c r="AU6" s="39"/>
       <c r="AV6" s="39"/>
       <c r="AW6" s="39"/>
@@ -1701,20 +2069,35 @@
     <row r="9" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9"/>
     </row>
-    <row r="10" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A10"/>
+      <c r="H10" s="69" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="11" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11"/>
-    </row>
-    <row r="12" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="H11" s="70" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="12" spans="1:66" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12"/>
+      <c r="H12" s="71" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="13" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13"/>
+      <c r="H13" s="72" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="14" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14"/>
+      <c r="H14" s="75" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="15" spans="1:66" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15"/>
@@ -1724,6 +2107,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="AZ1:BD1"/>
     <mergeCell ref="BE1:BI1"/>
     <mergeCell ref="BJ1:BN1"/>
     <mergeCell ref="V1:Z1"/>
@@ -1732,11 +2120,6 @@
     <mergeCell ref="AK1:AO1"/>
     <mergeCell ref="AP1:AT1"/>
     <mergeCell ref="AU1:AY1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="AZ1:BD1"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="8" scale="37" orientation="landscape" verticalDpi="300" r:id="rId1"/>
@@ -1748,8 +2131,8 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:Z39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="S9" sqref="S9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1773,10 +2156,10 @@
       <c r="B1" s="13">
         <v>13</v>
       </c>
-      <c r="C1" s="51">
+      <c r="C1" s="50">
         <v>14</v>
       </c>
-      <c r="D1" s="44">
+      <c r="D1" s="43">
         <v>15</v>
       </c>
       <c r="E1" s="13">
@@ -1804,7 +2187,7 @@
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B2" s="9"/>
       <c r="C2" s="9"/>
@@ -1826,13 +2209,13 @@
     </row>
     <row r="3" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B3" s="26"/>
-      <c r="C3" s="56"/>
+      <c r="C3" s="55"/>
       <c r="D3" s="38"/>
       <c r="E3" s="38"/>
-      <c r="F3" s="26"/>
+      <c r="F3" s="38"/>
       <c r="G3" s="8"/>
       <c r="H3" s="8"/>
       <c r="I3" s="8"/>
@@ -1840,7 +2223,7 @@
       <c r="K3" s="8"/>
       <c r="L3" s="15"/>
       <c r="U3" s="14" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="V3" s="24">
         <v>41019</v>
@@ -1848,14 +2231,13 @@
     </row>
     <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B4" s="26"/>
-      <c r="C4" s="56"/>
-      <c r="E4" s="49" t="s">
-        <v>56</v>
-      </c>
-      <c r="F4" s="26"/>
+      <c r="C4" s="55"/>
+      <c r="F4" s="48" t="s">
+        <v>55</v>
+      </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
       <c r="I4" s="8"/>
@@ -1863,7 +2245,7 @@
       <c r="K4" s="8"/>
       <c r="L4" s="15"/>
       <c r="U4" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="V4" s="24">
         <v>41026</v>
@@ -1874,13 +2256,13 @@
         <v>15</v>
       </c>
       <c r="B5" s="26"/>
-      <c r="C5" s="56"/>
+      <c r="C5" s="55"/>
       <c r="D5" s="36"/>
       <c r="E5" s="26"/>
-      <c r="F5" s="11" t="s">
+      <c r="F5" s="26"/>
+      <c r="G5" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="8"/>
       <c r="H5" s="8"/>
       <c r="I5" s="8"/>
       <c r="J5" s="8"/>
@@ -1892,39 +2274,40 @@
         <v>17</v>
       </c>
       <c r="B6" s="8"/>
-      <c r="C6" s="45"/>
+      <c r="C6" s="44"/>
       <c r="D6" s="36"/>
       <c r="E6" s="26"/>
       <c r="F6" s="26"/>
-      <c r="G6" s="9"/>
-      <c r="H6" s="26"/>
-      <c r="I6" s="26"/>
-      <c r="J6" s="26"/>
+      <c r="H6" s="9"/>
+      <c r="I6" s="9"/>
+      <c r="J6" s="9"/>
       <c r="K6" s="26"/>
       <c r="L6" s="15"/>
     </row>
     <row r="7" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B7" s="17"/>
-      <c r="C7" s="46"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="37"/>
       <c r="E7" s="30"/>
       <c r="F7" s="30"/>
       <c r="G7" s="17"/>
-      <c r="H7" s="30"/>
+      <c r="H7" s="17"/>
       <c r="I7" s="30"/>
-      <c r="J7" s="57"/>
-      <c r="K7" s="40"/>
+      <c r="J7" s="56"/>
+      <c r="K7" s="10" t="s">
+        <v>78</v>
+      </c>
       <c r="L7" s="19"/>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A8" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B8" s="21"/>
-      <c r="C8" s="47"/>
+      <c r="C8" s="46"/>
       <c r="D8" s="36"/>
       <c r="E8" s="31"/>
       <c r="F8" s="9"/>
@@ -1937,16 +2320,16 @@
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B9" s="8"/>
-      <c r="C9" s="45"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="36"/>
       <c r="E9" s="26"/>
       <c r="F9" s="26"/>
       <c r="G9" s="8"/>
-      <c r="I9" s="49" t="s">
-        <v>56</v>
+      <c r="I9" s="48" t="s">
+        <v>55</v>
       </c>
       <c r="J9" s="8"/>
       <c r="K9" s="8"/>
@@ -1957,7 +2340,7 @@
         <v>15</v>
       </c>
       <c r="B10" s="8"/>
-      <c r="C10" s="45"/>
+      <c r="C10" s="44"/>
       <c r="D10" s="36"/>
       <c r="E10" s="26"/>
       <c r="F10" s="26"/>
@@ -1975,7 +2358,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="8"/>
-      <c r="C11" s="45"/>
+      <c r="C11" s="44"/>
       <c r="D11" s="36"/>
       <c r="E11" s="26"/>
       <c r="F11" s="26"/>
@@ -1987,10 +2370,10 @@
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B12" s="8"/>
-      <c r="C12" s="45"/>
+      <c r="C12" s="44"/>
       <c r="D12" s="36"/>
       <c r="E12" s="26"/>
       <c r="F12" s="26"/>
@@ -1999,7 +2382,7 @@
       <c r="I12" s="8"/>
       <c r="J12" s="8"/>
       <c r="K12" s="10" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="L12" s="15"/>
     </row>
@@ -2007,9 +2390,9 @@
       <c r="A13" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="50"/>
-      <c r="C13" s="50"/>
-      <c r="D13" s="50"/>
+      <c r="B13" s="49"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
       <c r="G13" s="18"/>
@@ -2021,11 +2404,11 @@
     </row>
     <row r="14" spans="1:22" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="B14" s="50"/>
-      <c r="C14" s="50"/>
-      <c r="D14" s="50"/>
+        <v>61</v>
+      </c>
+      <c r="B14" s="49"/>
+      <c r="C14" s="49"/>
+      <c r="D14" s="49"/>
       <c r="E14" s="18"/>
       <c r="F14" s="18"/>
       <c r="G14" s="18"/>
@@ -2036,56 +2419,56 @@
       <c r="L14" s="19"/>
     </row>
     <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A15" s="41"/>
-      <c r="B15" s="42"/>
-      <c r="C15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
-      <c r="K15" s="42"/>
-      <c r="L15" s="41"/>
+      <c r="A15" s="40"/>
+      <c r="B15" s="41"/>
+      <c r="C15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
+      <c r="G15" s="41"/>
+      <c r="H15" s="41"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="40"/>
     </row>
     <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="42" t="s">
+      <c r="B16" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="C16" s="42" t="s">
+      <c r="C16" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="D16" s="42" t="s">
+      <c r="D16" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="F16" s="42" t="s">
+      <c r="F16" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="G16" s="42" t="s">
+      <c r="G16" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="H16" s="42" t="s">
+      <c r="H16" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="I16" s="42" t="s">
+      <c r="I16" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="J16" s="42" t="s">
+      <c r="J16" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="K16" s="42" t="s">
+      <c r="K16" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="L16" s="42" t="s">
+      <c r="L16" s="41" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B17">
         <v>10</v>
@@ -2160,25 +2543,25 @@
       <c r="D19">
         <v>80</v>
       </c>
-      <c r="E19" s="58">
+      <c r="E19" s="57">
         <v>90</v>
       </c>
-      <c r="F19" s="58">
+      <c r="F19" s="57">
         <v>80</v>
       </c>
-      <c r="G19" s="58">
+      <c r="G19" s="57">
         <v>73</v>
       </c>
-      <c r="H19" s="58">
+      <c r="H19" s="57">
         <v>100</v>
       </c>
-      <c r="I19" s="58">
+      <c r="I19" s="57">
         <v>80</v>
       </c>
-      <c r="J19" s="58">
+      <c r="J19" s="57">
         <v>70</v>
       </c>
-      <c r="K19" s="58"/>
+      <c r="K19" s="57"/>
       <c r="L19" s="29"/>
       <c r="M19" s="29"/>
       <c r="N19" s="29"/>
@@ -2191,7 +2574,7 @@
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C20">
         <v>40</v>
@@ -2290,48 +2673,48 @@
       <c r="B25" s="28"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A30" s="41"/>
-      <c r="B30" s="41"/>
-      <c r="C30" s="41"/>
-      <c r="D30" s="42" t="s">
+      <c r="A30" s="40"/>
+      <c r="B30" s="40"/>
+      <c r="C30" s="40"/>
+      <c r="D30" s="41" t="s">
         <v>31</v>
       </c>
-      <c r="E30" s="42" t="s">
+      <c r="E30" s="41" t="s">
         <v>32</v>
       </c>
-      <c r="F30" s="42" t="s">
+      <c r="F30" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="G30" s="42" t="s">
+      <c r="G30" s="41" t="s">
         <v>34</v>
       </c>
-      <c r="H30" s="42" t="s">
+      <c r="H30" s="41" t="s">
         <v>35</v>
       </c>
-      <c r="I30" s="42" t="s">
+      <c r="I30" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="J30" s="42" t="s">
+      <c r="J30" s="41" t="s">
         <v>37</v>
       </c>
-      <c r="K30" s="42" t="s">
+      <c r="K30" s="41" t="s">
         <v>38</v>
       </c>
-      <c r="L30" s="42" t="s">
+      <c r="L30" s="41" t="s">
         <v>39</v>
       </c>
-      <c r="M30" s="42" t="s">
+      <c r="M30" s="41" t="s">
         <v>40</v>
       </c>
-      <c r="N30" s="42" t="s">
+      <c r="N30" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="O30" s="41"/>
-      <c r="P30" s="41"/>
-      <c r="Q30" s="41"/>
+      <c r="O30" s="40"/>
+      <c r="P30" s="40"/>
+      <c r="Q30" s="40"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="42" t="s">
         <v>30</v>
       </c>
       <c r="B31" s="28" t="s">
@@ -2343,7 +2726,7 @@
         <v>49</v>
       </c>
       <c r="B32" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="F32">
         <v>30</v>
@@ -2378,20 +2761,20 @@
       <c r="F33">
         <v>20</v>
       </c>
-      <c r="G33" s="58">
+      <c r="G33" s="57">
         <v>30</v>
       </c>
-      <c r="H33" s="58"/>
-      <c r="I33" s="58">
+      <c r="H33" s="57"/>
+      <c r="I33" s="57">
         <v>33</v>
       </c>
-      <c r="J33" s="58">
+      <c r="J33" s="57">
         <v>30</v>
       </c>
-      <c r="K33" s="58">
+      <c r="K33" s="57">
         <v>20</v>
       </c>
-      <c r="L33" s="58">
+      <c r="L33" s="57">
         <v>10</v>
       </c>
       <c r="R33">
@@ -2476,7 +2859,7 @@
         <v>21</v>
       </c>
       <c r="B36" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D36">
         <v>10</v>
@@ -2494,7 +2877,7 @@
         <v>22</v>
       </c>
       <c r="B37" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G37">
         <v>10</v>
@@ -2512,7 +2895,7 @@
         <v>18</v>
       </c>
       <c r="B38" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E38">
         <v>40</v>

</xml_diff>